<commit_message>
update of repository structure and data product 3.
</commit_message>
<xml_diff>
--- a/Permit Data Inventory/BuildingPermitDataInventory_Wyman_2025mmdd_v3.xlsx
+++ b/Permit Data Inventory/BuildingPermitDataInventory_Wyman_2025mmdd_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukewyman/github-classroom/bmkt699-capstone-2025spring/capstone_missoula_building_permits/Permit Data Inventory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED108541-6416-794D-AE5B-BCE3108F617D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6882E1-DC6C-074A-977C-0E5BA73840B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="22100" windowWidth="38400" windowHeight="19760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Requirements" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="201">
   <si>
     <t>Permit ID</t>
   </si>
@@ -1049,6 +1049,15 @@
   </si>
   <si>
     <t>In applicant's hands</t>
+  </si>
+  <si>
+    <t>FINAL</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>After Inspection</t>
   </si>
 </sst>
 </file>
@@ -3816,7 +3825,7 @@
   <dimension ref="A1:M998"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
@@ -7224,10 +7233,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D0EFCE-BAB4-DF48-99B7-DBB4E3025014}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7482,6 +7491,28 @@
         <v>197</v>
       </c>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7491,8 +7522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF86347D-13E8-7246-AE31-E15D2D93ED2D}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="161" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="161" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -7501,7 +7532,7 @@
     <col min="2" max="2" width="17.796875" customWidth="1"/>
     <col min="3" max="4" width="31.3984375" customWidth="1"/>
     <col min="5" max="5" width="32.19921875" customWidth="1"/>
-    <col min="6" max="6" width="44.19921875" customWidth="1"/>
+    <col min="6" max="6" width="69.59765625" customWidth="1"/>
     <col min="7" max="7" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.59765625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
@@ -7562,7 +7593,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="143" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>101</v>
       </c>

</xml_diff>